<commit_message>
Updated datasets to include full Lake Florida sample
</commit_message>
<xml_diff>
--- a/Data/Season2/Encounters - Double observer - distance survey (Responses).xlsx
+++ b/Data/Season2/Encounters - Double observer - distance survey (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="46">
   <si>
     <t>Timestamp</t>
   </si>
@@ -141,6 +141,15 @@
   <si>
     <t>Can</t>
   </si>
+  <si>
+    <t>on dead shell</t>
+  </si>
+  <si>
+    <t>No mussels</t>
+  </si>
+  <si>
+    <t>0 mussels</t>
+  </si>
 </sst>
 </file>
 
@@ -12979,6 +12988,851 @@
         <v>33</v>
       </c>
     </row>
+    <row r="348">
+      <c r="A348" s="2">
+        <v>43314.50230461806</v>
+      </c>
+      <c r="B348" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E348" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F348" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="G348" s="1">
+        <v>82.0</v>
+      </c>
+      <c r="H348" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I348" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J348" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="K348" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L348" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="2">
+        <v>43314.50268737269</v>
+      </c>
+      <c r="B349" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E349" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F349" s="1">
+        <v>14.52</v>
+      </c>
+      <c r="G349" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="H349" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I349" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J349" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="K349" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="L349" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="2">
+        <v>43314.50307409722</v>
+      </c>
+      <c r="B350" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E350" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F350" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="G350" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="H350" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I350" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J350" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="K350" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="L350" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="2">
+        <v>43314.50361134259</v>
+      </c>
+      <c r="B351" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E351" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="F351" s="1">
+        <v>19.41</v>
+      </c>
+      <c r="G351" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="H351" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I351" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J351" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="K351" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="L351" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M351" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="2">
+        <v>43314.506624629634</v>
+      </c>
+      <c r="B352" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E352" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="M352" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="2">
+        <v>43314.50792142361</v>
+      </c>
+      <c r="B353" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E353" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="F353" s="1">
+        <v>3.45</v>
+      </c>
+      <c r="G353" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="H353" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I353" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J353" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="K353" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L353" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="2">
+        <v>43314.50824556713</v>
+      </c>
+      <c r="B354" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E354" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="F354" s="1">
+        <v>5.31</v>
+      </c>
+      <c r="G354" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="H354" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I354" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J354" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="K354" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L354" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="2">
+        <v>43314.508628125</v>
+      </c>
+      <c r="B355" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E355" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="F355" s="1">
+        <v>13.18</v>
+      </c>
+      <c r="G355" s="1">
+        <v>28.0</v>
+      </c>
+      <c r="H355" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I355" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J355" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="K355" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L355" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="2">
+        <v>43314.50901388889</v>
+      </c>
+      <c r="B356" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E356" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="F356" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="G356" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="H356" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I356" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J356" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="K356" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L356" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="2">
+        <v>43314.51064493056</v>
+      </c>
+      <c r="B357" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E357" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F357" s="1">
+        <v>3.45</v>
+      </c>
+      <c r="G357" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="H357" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I357" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J357" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="K357" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="L357" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="2">
+        <v>43314.51115289352</v>
+      </c>
+      <c r="B358" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E358" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F358" s="1">
+        <v>5.12</v>
+      </c>
+      <c r="G358" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="H358" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I358" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J358" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="K358" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="L358" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="2">
+        <v>43314.51164375</v>
+      </c>
+      <c r="B359" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E359" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F359" s="1">
+        <v>8.02</v>
+      </c>
+      <c r="G359" s="1">
+        <v>98.0</v>
+      </c>
+      <c r="H359" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I359" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J359" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="K359" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L359" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="2">
+        <v>43314.5122212037</v>
+      </c>
+      <c r="B360" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E360" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F360" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="G360" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="H360" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I360" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J360" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="K360" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="L360" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="2">
+        <v>43314.512673136574</v>
+      </c>
+      <c r="B361" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E361" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F361" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="G361" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="H361" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I361" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J361" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="K361" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="L361" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="2">
+        <v>43314.51318565972</v>
+      </c>
+      <c r="B362" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E362" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F362" s="1">
+        <v>15.45</v>
+      </c>
+      <c r="G362" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="H362" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I362" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J362" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="K362" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="L362" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="2">
+        <v>43314.51356288194</v>
+      </c>
+      <c r="B363" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E363" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F363" s="1">
+        <v>16.85</v>
+      </c>
+      <c r="G363" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H363" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I363" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J363" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="K363" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="L363" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="2">
+        <v>43314.5139537037</v>
+      </c>
+      <c r="B364" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E364" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F364" s="1">
+        <v>17.08</v>
+      </c>
+      <c r="G364" s="1">
+        <v>93.0</v>
+      </c>
+      <c r="H364" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I364" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J364" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="K364" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="L364" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="2">
+        <v>43314.514324143514</v>
+      </c>
+      <c r="B365" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E365" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F365" s="1">
+        <v>18.1</v>
+      </c>
+      <c r="G365" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="H365" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I365" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J365" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="K365" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="L365" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="2">
+        <v>43314.514644826384</v>
+      </c>
+      <c r="B366" s="3">
+        <v>43313.0</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E366" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="F366" s="1">
+        <v>19.18</v>
+      </c>
+      <c r="G366" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="H366" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I366" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J366" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="K366" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="L366" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="2">
+        <v>43328.49418869213</v>
+      </c>
+      <c r="B367" s="3">
+        <v>43326.0</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E367" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="M367" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="2">
+        <v>43328.49526739583</v>
+      </c>
+      <c r="B368" s="3">
+        <v>43326.0</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D368" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E368" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="M368" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="2">
+        <v>43328.4956521875</v>
+      </c>
+      <c r="B369" s="3">
+        <v>43326.0</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D369" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E369" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="M369" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="2">
+        <v>43328.54446502315</v>
+      </c>
+      <c r="B370" s="3">
+        <v>43326.0</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E370" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="I370" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="2">
+        <v>43328.54477920139</v>
+      </c>
+      <c r="B371" s="3">
+        <v>43326.0</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E371" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="F371" s="1">
+        <v>3.27</v>
+      </c>
+      <c r="G371" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="H371" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I371" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J371" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="K371" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L371" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="2">
+        <v>43328.54500013889</v>
+      </c>
+      <c r="B372" s="3">
+        <v>43326.0</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E372" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="I372" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>